<commit_message>
update mocklist + PPP
</commit_message>
<xml_diff>
--- a/studies/labor study_A/study1_mocklist.xlsx
+++ b/studies/labor study_A/study1_mocklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mk99feta\Documents\GitHub\Mandy-PhD\studies\labor study_A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CD840E-0A96-44B9-A8CB-BF879431868F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0331444A-46F5-40B8-972E-06656DD00CAB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" tabRatio="661" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" tabRatio="661" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="subject_list" sheetId="8" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1952" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2286" uniqueCount="352">
   <si>
     <t>study</t>
   </si>
@@ -1058,6 +1058,33 @@
   </si>
   <si>
     <t>personD</t>
+  </si>
+  <si>
+    <t>social studies</t>
+  </si>
+  <si>
+    <t>no cam 1</t>
+  </si>
+  <si>
+    <t>uni</t>
+  </si>
+  <si>
+    <t>educational studies</t>
+  </si>
+  <si>
+    <t>philosophy</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>lack_staring</t>
+  </si>
+  <si>
+    <t>(agit_walk)</t>
   </si>
 </sst>
 </file>
@@ -1354,7 +1381,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="27">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1507,6 +1534,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1691,7 +1724,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="184">
+  <cellXfs count="192">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2054,6 +2087,20 @@
     <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
@@ -2451,8 +2498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2462,8 +2509,10 @@
     <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.26953125" style="11" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="4.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="14.54296875" customWidth="1"/>
+    <col min="6" max="6" width="4.1796875" customWidth="1"/>
+    <col min="7" max="7" width="14.54296875" customWidth="1"/>
+    <col min="8" max="8" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.54296875" customWidth="1"/>
     <col min="10" max="10" width="14.7265625" customWidth="1"/>
     <col min="11" max="11" width="10.81640625" customWidth="1"/>
     <col min="12" max="12" width="14.54296875" customWidth="1"/>
@@ -2564,354 +2613,354 @@
       </c>
     </row>
     <row r="2" spans="1:27" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="184">
+        <v>1</v>
+      </c>
+      <c r="B2" s="184" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="184" t="s">
         <v>47</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="186" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="7">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="G2" s="184" t="s">
         <v>105</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="184" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="3">
-        <v>15</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K2" s="3" t="s">
+      <c r="I2" s="184">
+        <v>25</v>
+      </c>
+      <c r="J2" s="184" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="184" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="184" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="N2" s="3">
+      <c r="M2" s="185" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" s="184">
         <v>21</v>
       </c>
-      <c r="O2" s="3">
+      <c r="O2" s="184">
         <v>2</v>
       </c>
-      <c r="P2" s="3">
+      <c r="P2" s="184">
         <v>1969</v>
       </c>
-      <c r="Q2" s="3" t="str">
+      <c r="Q2" s="184" t="str">
         <f t="shared" ref="Q2" si="0">N2&amp;"/"&amp;O2&amp;"/"&amp;P2</f>
         <v>21/2/1969</v>
       </c>
-      <c r="R2" s="3">
+      <c r="R2" s="184">
         <v>29</v>
       </c>
-      <c r="S2" s="3">
+      <c r="S2" s="184">
         <v>7</v>
       </c>
-      <c r="T2" s="3">
+      <c r="T2" s="184">
         <v>2020</v>
       </c>
-      <c r="U2" s="3" t="str">
+      <c r="U2" s="184" t="str">
         <f>R2&amp;"/"&amp;S2&amp;"/"&amp;T2</f>
         <v>29/7/2020</v>
       </c>
-      <c r="V2" s="3">
+      <c r="V2" s="184">
         <f t="shared" ref="V2" si="1">DATEDIF(Q2, U2, "m")</f>
         <v>617</v>
       </c>
-      <c r="W2" s="3">
+      <c r="W2" s="184">
         <f t="shared" ref="W2" si="2">DATEDIF(Q2, U2, "d")</f>
         <v>18786</v>
       </c>
-      <c r="X2" s="3">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="3" t="str">
+      <c r="X2" s="184">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="184">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="184" t="str">
         <f>CONCATENATE(B2,"_",C2,D2,"_",E2)</f>
         <v>Study1_pilot01_expert</v>
       </c>
-      <c r="AA2" s="3" t="s">
-        <v>13</v>
+      <c r="AA2" s="184" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:27" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
+      <c r="A3" s="184">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="184" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="184" t="s">
         <v>47</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="186" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="5">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="F3" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="G3" s="184" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="I3" s="3">
-        <v>9</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K3" s="3" t="s">
+      <c r="H3" s="184" t="s">
+        <v>343</v>
+      </c>
+      <c r="I3" s="184">
+        <v>15</v>
+      </c>
+      <c r="J3" s="184" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="184" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="184" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N3" s="3">
+      <c r="M3" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="184">
         <v>20</v>
       </c>
-      <c r="O3" s="3">
+      <c r="O3" s="184">
         <v>12</v>
       </c>
-      <c r="P3" s="3">
+      <c r="P3" s="184">
         <v>1975</v>
       </c>
-      <c r="Q3" s="3" t="str">
+      <c r="Q3" s="184" t="str">
         <f t="shared" ref="Q3:Q6" si="3">N3&amp;"/"&amp;O3&amp;"/"&amp;P3</f>
         <v>20/12/1975</v>
       </c>
-      <c r="R3" s="3">
+      <c r="R3" s="184">
         <v>29</v>
       </c>
-      <c r="S3" s="3">
+      <c r="S3" s="184">
         <v>7</v>
       </c>
-      <c r="T3" s="3">
+      <c r="T3" s="184">
         <v>2020</v>
       </c>
-      <c r="U3" s="3" t="str">
+      <c r="U3" s="184" t="str">
         <f t="shared" ref="U3:U6" si="4">R3&amp;"/"&amp;S3&amp;"/"&amp;T3</f>
         <v>29/7/2020</v>
       </c>
-      <c r="V3" s="3">
+      <c r="V3" s="184">
         <f t="shared" ref="V3:V13" si="5">DATEDIF(Q3, U3, "m")</f>
         <v>535</v>
       </c>
-      <c r="W3" s="3">
+      <c r="W3" s="184">
         <f t="shared" ref="W3:W13" si="6">DATEDIF(Q3, U3, "d")</f>
         <v>16293</v>
       </c>
-      <c r="X3" s="3">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="3" t="str">
+      <c r="X3" s="184">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="184">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="184" t="str">
         <f t="shared" ref="Z3:Z13" si="7">CONCATENATE(B3,"_",C3,D3,"_",E3)</f>
         <v>Study1_pilot01_expert</v>
       </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AA3" s="184" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:27" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
+      <c r="A4" s="184">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="184" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="184" t="s">
         <v>47</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>45</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="I4" s="3">
-        <v>12</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="G4" s="184" t="s">
+        <v>345</v>
+      </c>
+      <c r="H4" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I4" s="184">
+        <v>1.5</v>
+      </c>
+      <c r="J4" s="184" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="184" t="s">
         <v>31</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="184" t="s">
         <v>41</v>
       </c>
-      <c r="M4" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="N4" s="3">
+      <c r="M4" s="185" t="s">
+        <v>37</v>
+      </c>
+      <c r="N4" s="184">
         <v>15</v>
       </c>
-      <c r="O4" s="3">
-        <v>1</v>
-      </c>
-      <c r="P4" s="3">
+      <c r="O4" s="184">
+        <v>1</v>
+      </c>
+      <c r="P4" s="184">
         <v>1991</v>
       </c>
-      <c r="Q4" s="3" t="str">
+      <c r="Q4" s="184" t="str">
         <f t="shared" si="3"/>
         <v>15/1/1991</v>
       </c>
-      <c r="R4" s="3">
+      <c r="R4" s="184">
         <v>29</v>
       </c>
-      <c r="S4" s="3">
+      <c r="S4" s="184">
         <v>7</v>
       </c>
-      <c r="T4" s="3">
+      <c r="T4" s="184">
         <v>2020</v>
       </c>
-      <c r="U4" s="3" t="str">
+      <c r="U4" s="184" t="str">
         <f t="shared" si="4"/>
         <v>29/7/2020</v>
       </c>
-      <c r="V4" s="3">
+      <c r="V4" s="184">
         <f t="shared" si="5"/>
         <v>354</v>
       </c>
-      <c r="W4" s="3">
+      <c r="W4" s="184">
         <f t="shared" si="6"/>
         <v>10788</v>
       </c>
-      <c r="X4" s="3">
-        <v>1</v>
-      </c>
-      <c r="Y4" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="3" t="str">
+      <c r="X4" s="184">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="184">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="184" t="str">
         <f t="shared" si="7"/>
-        <v>Study1_pilot01_expert</v>
-      </c>
-      <c r="AA4" s="3" t="s">
+        <v>Study1_pilot01_novice</v>
+      </c>
+      <c r="AA4" s="184" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:27" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
+      <c r="A5" s="184">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="184" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="184" t="s">
         <v>47</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="7">
-        <v>1</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="I5" s="3">
-        <v>14</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="G5" s="184" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="184" t="s">
+        <v>347</v>
+      </c>
+      <c r="I5" s="184">
+        <v>0.6</v>
+      </c>
+      <c r="J5" s="184" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="184" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="184" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="N5" s="3">
+      <c r="M5" s="185" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" s="184">
         <v>23</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5" s="184">
         <v>3</v>
       </c>
-      <c r="P5" s="3">
+      <c r="P5" s="184">
         <v>1993</v>
       </c>
-      <c r="Q5" s="3" t="str">
+      <c r="Q5" s="184" t="str">
         <f t="shared" si="3"/>
         <v>23/3/1993</v>
       </c>
-      <c r="R5" s="3">
+      <c r="R5" s="184">
         <v>29</v>
       </c>
-      <c r="S5" s="3">
+      <c r="S5" s="184">
         <v>7</v>
       </c>
-      <c r="T5" s="3">
+      <c r="T5" s="184">
         <v>2020</v>
       </c>
-      <c r="U5" s="3" t="str">
+      <c r="U5" s="184" t="str">
         <f t="shared" si="4"/>
         <v>29/7/2020</v>
       </c>
-      <c r="V5" s="3">
+      <c r="V5" s="184">
         <f t="shared" si="5"/>
         <v>328</v>
       </c>
-      <c r="W5" s="3">
+      <c r="W5" s="184">
         <f t="shared" si="6"/>
         <v>9990</v>
       </c>
-      <c r="X5" s="3">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z5" s="3" t="str">
+      <c r="X5" s="184">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="184">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="184" t="str">
         <f t="shared" si="7"/>
-        <v>Study1_pilot01_expert</v>
-      </c>
-      <c r="AA5" s="3" t="s">
+        <v>Study1_pilot01_novice</v>
+      </c>
+      <c r="AA5" s="184" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2931,8 +2980,8 @@
       <c r="E6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="7">
-        <v>1</v>
+      <c r="F6" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>62</v>
@@ -3019,8 +3068,8 @@
       <c r="E7" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="5">
-        <v>0</v>
+      <c r="F7" s="5" t="s">
+        <v>349</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>62</v>
@@ -3107,8 +3156,8 @@
       <c r="E8" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="5">
-        <v>0</v>
+      <c r="F8" s="5" t="s">
+        <v>349</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>62</v>
@@ -3195,8 +3244,8 @@
       <c r="E9" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="7">
-        <v>1</v>
+      <c r="F9" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>62</v>
@@ -3283,8 +3332,8 @@
       <c r="E10" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="5">
-        <v>0</v>
+      <c r="F10" s="5" t="s">
+        <v>349</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>63</v>
@@ -3371,8 +3420,8 @@
       <c r="E11" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="7">
-        <v>1</v>
+      <c r="F11" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>61</v>
@@ -3459,8 +3508,8 @@
       <c r="E12" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="5">
-        <v>0</v>
+      <c r="F12" s="5" t="s">
+        <v>349</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>61</v>
@@ -3547,8 +3596,8 @@
       <c r="E13" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="5">
-        <v>0</v>
+      <c r="F13" s="5" t="s">
+        <v>349</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>61</v>
@@ -10441,11 +10490,11 @@
       <c r="M56" s="112"/>
       <c r="O56">
         <f ca="1">RANDBETWEEN(1,11)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="Q56">
         <f ca="1">RANDBETWEEN(1,11)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.35">
@@ -10468,7 +10517,7 @@
       </c>
       <c r="Q57">
         <f t="shared" ref="Q57:Q66" ca="1" si="1">RANDBETWEEN(1,11)</f>
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.35">
@@ -10484,11 +10533,11 @@
       <c r="M58" s="112"/>
       <c r="O58">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Q58">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.35">
@@ -10504,7 +10553,7 @@
       <c r="M59" s="112"/>
       <c r="O59">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="Q59">
         <f t="shared" ca="1" si="1"/>
@@ -10527,11 +10576,11 @@
       <c r="M60" s="112"/>
       <c r="O60">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q60">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.35">
@@ -10559,11 +10608,11 @@
       <c r="M61" s="112"/>
       <c r="O61">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="Q61">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.35">
@@ -10591,11 +10640,11 @@
       <c r="M62" s="112"/>
       <c r="O62">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="Q62">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.35">
@@ -10621,11 +10670,11 @@
       <c r="M63" s="112"/>
       <c r="O63">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="Q63">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.35">
@@ -10651,11 +10700,11 @@
       <c r="M64" s="112"/>
       <c r="O64">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="Q64">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.35">
@@ -10677,7 +10726,7 @@
       </c>
       <c r="Q65">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.35">
@@ -10693,11 +10742,11 @@
       <c r="M66" s="112"/>
       <c r="O66">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q66">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.35">
@@ -10987,8 +11036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93E918F0-9C6B-4528-8541-240528FAF3FE}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11044,8 +11093,8 @@
       <c r="D3" s="118" t="s">
         <v>270</v>
       </c>
-      <c r="E3" s="26" t="s">
-        <v>273</v>
+      <c r="E3" s="188" t="s">
+        <v>351</v>
       </c>
       <c r="I3"/>
     </row>
@@ -11057,7 +11106,7 @@
       <c r="C4" s="119" t="s">
         <v>268</v>
       </c>
-      <c r="D4" s="119" t="s">
+      <c r="D4" s="118" t="s">
         <v>271</v>
       </c>
       <c r="E4" s="92" t="s">
@@ -11067,436 +11116,431 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B5" s="11"/>
+      <c r="D5" s="191" t="s">
+        <v>350</v>
+      </c>
       <c r="I5"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="130" t="s">
-        <v>282</v>
-      </c>
-      <c r="B6" s="125"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="120"/>
-      <c r="I6"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="131"/>
-      <c r="B7" s="123"/>
-      <c r="C7" s="118"/>
-      <c r="D7" s="118"/>
-      <c r="E7" s="118"/>
-      <c r="F7" s="26"/>
-      <c r="I7"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="130" t="s">
-        <v>283</v>
-      </c>
-      <c r="B8" s="126"/>
-      <c r="C8" s="133" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="133" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="133" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="134" t="s">
-        <v>39</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="B8" s="125"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="120"/>
       <c r="I8"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="131"/>
-      <c r="B9" s="128" t="s">
-        <v>275</v>
-      </c>
-      <c r="C9" s="116"/>
-      <c r="D9" s="116"/>
-      <c r="E9" s="116"/>
-      <c r="F9" s="117"/>
+      <c r="B9" s="123"/>
+      <c r="C9" s="118"/>
+      <c r="D9" s="118"/>
+      <c r="E9" s="118"/>
+      <c r="F9" s="26"/>
       <c r="I9"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="131"/>
-      <c r="B10" s="124" t="s">
-        <v>276</v>
-      </c>
-      <c r="C10" s="121" t="s">
-        <v>279</v>
-      </c>
-      <c r="D10" s="118" t="s">
-        <v>272</v>
-      </c>
-      <c r="E10" s="118" t="s">
-        <v>267</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>271</v>
+      <c r="A10" s="130" t="s">
+        <v>283</v>
+      </c>
+      <c r="B10" s="126"/>
+      <c r="C10" s="133" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="133" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="133" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="134" t="s">
+        <v>39</v>
       </c>
       <c r="I10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="131"/>
-      <c r="B11" s="124" t="s">
-        <v>277</v>
-      </c>
-      <c r="C11" s="121" t="s">
-        <v>279</v>
-      </c>
-      <c r="D11" s="118" t="s">
-        <v>269</v>
-      </c>
-      <c r="E11" s="118" t="s">
-        <v>273</v>
-      </c>
-      <c r="F11" s="26" t="s">
-        <v>268</v>
-      </c>
+      <c r="B11" s="128" t="s">
+        <v>275</v>
+      </c>
+      <c r="C11" s="116"/>
+      <c r="D11" s="116"/>
+      <c r="E11" s="116"/>
+      <c r="F11" s="117"/>
       <c r="I11"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="131"/>
-      <c r="B12" s="127" t="s">
-        <v>278</v>
-      </c>
-      <c r="C12" s="122" t="s">
+      <c r="B12" s="124" t="s">
+        <v>276</v>
+      </c>
+      <c r="C12" s="121" t="s">
         <v>279</v>
       </c>
-      <c r="D12" s="119" t="s">
-        <v>266</v>
-      </c>
-      <c r="E12" s="119" t="s">
-        <v>270</v>
-      </c>
-      <c r="F12" s="92" t="s">
-        <v>274</v>
+      <c r="D12" s="118" t="s">
+        <v>272</v>
+      </c>
+      <c r="E12" s="118" t="s">
+        <v>267</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>271</v>
       </c>
       <c r="I12"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="131"/>
-      <c r="B13" s="124"/>
-      <c r="C13" s="118"/>
-      <c r="D13" s="118"/>
-      <c r="E13" s="118"/>
-      <c r="F13" s="26"/>
+      <c r="B13" s="124" t="s">
+        <v>277</v>
+      </c>
+      <c r="C13" s="121" t="s">
+        <v>279</v>
+      </c>
+      <c r="D13" s="118" t="s">
+        <v>269</v>
+      </c>
+      <c r="E13" s="187" t="s">
+        <v>350</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>268</v>
+      </c>
       <c r="I13"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="131"/>
-      <c r="B14" s="124"/>
-      <c r="C14" s="118"/>
-      <c r="D14" s="118"/>
-      <c r="E14" s="118"/>
-      <c r="F14" s="26"/>
+      <c r="B14" s="127" t="s">
+        <v>278</v>
+      </c>
+      <c r="C14" s="122" t="s">
+        <v>279</v>
+      </c>
+      <c r="D14" s="119" t="s">
+        <v>266</v>
+      </c>
+      <c r="E14" s="119" t="s">
+        <v>270</v>
+      </c>
+      <c r="F14" s="92" t="s">
+        <v>274</v>
+      </c>
       <c r="I14"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="130" t="s">
-        <v>284</v>
-      </c>
-      <c r="B15" s="126"/>
-      <c r="C15" s="133" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="133" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="133" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="134" t="s">
-        <v>39</v>
-      </c>
+      <c r="A15" s="131"/>
+      <c r="B15" s="124"/>
+      <c r="C15" s="118"/>
+      <c r="D15" s="118"/>
+      <c r="E15" s="118"/>
+      <c r="F15" s="26"/>
       <c r="I15"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="131"/>
-      <c r="B16" s="128" t="s">
-        <v>275</v>
-      </c>
-      <c r="C16" s="116"/>
-      <c r="D16" s="116"/>
-      <c r="E16" s="116"/>
-      <c r="F16" s="117"/>
+      <c r="B16" s="124"/>
+      <c r="C16" s="118"/>
+      <c r="D16" s="118"/>
+      <c r="E16" s="118"/>
+      <c r="F16" s="26"/>
       <c r="I16"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="131"/>
-      <c r="B17" s="124" t="s">
-        <v>276</v>
-      </c>
-      <c r="C17" s="118" t="s">
-        <v>274</v>
-      </c>
-      <c r="D17" s="121" t="s">
-        <v>279</v>
-      </c>
-      <c r="E17" s="118" t="s">
-        <v>269</v>
-      </c>
-      <c r="F17" s="26" t="s">
-        <v>267</v>
+      <c r="A17" s="130" t="s">
+        <v>284</v>
+      </c>
+      <c r="B17" s="126"/>
+      <c r="C17" s="133" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="133" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="133" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="134" t="s">
+        <v>39</v>
       </c>
       <c r="I17"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="131"/>
-      <c r="B18" s="124" t="s">
-        <v>277</v>
-      </c>
-      <c r="C18" s="118" t="s">
-        <v>268</v>
-      </c>
-      <c r="D18" s="121" t="s">
-        <v>279</v>
-      </c>
-      <c r="E18" s="118" t="s">
-        <v>272</v>
-      </c>
-      <c r="F18" s="26" t="s">
-        <v>270</v>
-      </c>
+      <c r="B18" s="128" t="s">
+        <v>275</v>
+      </c>
+      <c r="C18" s="116"/>
+      <c r="D18" s="116"/>
+      <c r="E18" s="116"/>
+      <c r="F18" s="117"/>
       <c r="I18"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="131"/>
-      <c r="B19" s="127" t="s">
-        <v>278</v>
-      </c>
-      <c r="C19" s="119" t="s">
-        <v>271</v>
-      </c>
-      <c r="D19" s="122" t="s">
+      <c r="B19" s="124" t="s">
+        <v>276</v>
+      </c>
+      <c r="C19" s="118" t="s">
+        <v>274</v>
+      </c>
+      <c r="D19" s="121" t="s">
         <v>279</v>
       </c>
-      <c r="E19" s="119" t="s">
-        <v>266</v>
-      </c>
-      <c r="F19" s="92" t="s">
-        <v>273</v>
+      <c r="E19" s="118" t="s">
+        <v>269</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>267</v>
       </c>
       <c r="I19"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="131"/>
-      <c r="B20" s="124"/>
-      <c r="C20" s="118"/>
-      <c r="D20" s="118"/>
-      <c r="E20" s="118"/>
-      <c r="F20" s="26"/>
+      <c r="B20" s="124" t="s">
+        <v>277</v>
+      </c>
+      <c r="C20" s="118" t="s">
+        <v>268</v>
+      </c>
+      <c r="D20" s="121" t="s">
+        <v>279</v>
+      </c>
+      <c r="E20" s="118" t="s">
+        <v>272</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>270</v>
+      </c>
       <c r="I20"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="131"/>
-      <c r="B21" s="124"/>
-      <c r="C21" s="118"/>
-      <c r="D21" s="118"/>
-      <c r="E21" s="118"/>
-      <c r="F21" s="26"/>
+      <c r="B21" s="127" t="s">
+        <v>278</v>
+      </c>
+      <c r="C21" s="119" t="s">
+        <v>271</v>
+      </c>
+      <c r="D21" s="122" t="s">
+        <v>279</v>
+      </c>
+      <c r="E21" s="119" t="s">
+        <v>266</v>
+      </c>
+      <c r="F21" s="189" t="s">
+        <v>350</v>
+      </c>
       <c r="I21"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="130" t="s">
-        <v>285</v>
-      </c>
-      <c r="B22" s="126"/>
-      <c r="C22" s="133" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="133" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="133" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" s="134" t="s">
-        <v>39</v>
-      </c>
+      <c r="A22" s="131"/>
+      <c r="B22" s="124"/>
+      <c r="C22" s="118"/>
+      <c r="D22" s="118"/>
+      <c r="E22" s="118"/>
+      <c r="F22" s="26"/>
       <c r="I22"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="131"/>
-      <c r="B23" s="128" t="s">
-        <v>275</v>
-      </c>
-      <c r="C23" s="116"/>
-      <c r="D23" s="116"/>
-      <c r="E23" s="116"/>
-      <c r="F23" s="117"/>
+      <c r="B23" s="124"/>
+      <c r="C23" s="118"/>
+      <c r="D23" s="118"/>
+      <c r="E23" s="118"/>
+      <c r="F23" s="26"/>
       <c r="I23"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="131"/>
-      <c r="B24" s="124" t="s">
-        <v>276</v>
-      </c>
-      <c r="C24" s="118" t="s">
-        <v>267</v>
-      </c>
-      <c r="D24" s="118" t="s">
-        <v>274</v>
-      </c>
-      <c r="E24" s="121" t="s">
-        <v>279</v>
-      </c>
-      <c r="F24" s="26" t="s">
-        <v>269</v>
+      <c r="A24" s="130" t="s">
+        <v>285</v>
+      </c>
+      <c r="B24" s="126"/>
+      <c r="C24" s="133" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="133" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="133" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" s="134" t="s">
+        <v>39</v>
       </c>
       <c r="I24"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="131"/>
-      <c r="B25" s="124" t="s">
+      <c r="B25" s="128" t="s">
+        <v>275</v>
+      </c>
+      <c r="C25" s="116"/>
+      <c r="D25" s="116"/>
+      <c r="E25" s="116"/>
+      <c r="F25" s="117"/>
+      <c r="I25"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="131"/>
+      <c r="B26" s="124" t="s">
+        <v>276</v>
+      </c>
+      <c r="C26" s="118" t="s">
+        <v>267</v>
+      </c>
+      <c r="D26" s="118" t="s">
+        <v>274</v>
+      </c>
+      <c r="E26" s="121" t="s">
+        <v>279</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="I26"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="131"/>
+      <c r="B27" s="124" t="s">
         <v>277</v>
       </c>
-      <c r="C25" s="118" t="s">
+      <c r="C27" s="118" t="s">
         <v>270</v>
       </c>
-      <c r="D25" s="118" t="s">
+      <c r="D27" s="118" t="s">
         <v>268</v>
       </c>
-      <c r="E25" s="121" t="s">
+      <c r="E27" s="121" t="s">
         <v>279</v>
       </c>
-      <c r="F25" s="26" t="s">
+      <c r="F27" s="26" t="s">
         <v>272</v>
       </c>
-      <c r="I25"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="132"/>
-      <c r="B26" s="127" t="s">
+      <c r="I27"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="132"/>
+      <c r="B28" s="127" t="s">
         <v>278</v>
       </c>
-      <c r="C26" s="119" t="s">
-        <v>273</v>
-      </c>
-      <c r="D26" s="119" t="s">
+      <c r="C28" s="190" t="s">
+        <v>350</v>
+      </c>
+      <c r="D28" s="119" t="s">
         <v>271</v>
       </c>
-      <c r="E26" s="122" t="s">
+      <c r="E28" s="122" t="s">
         <v>279</v>
       </c>
-      <c r="F26" s="92" t="s">
+      <c r="F28" s="92" t="s">
         <v>266</v>
       </c>
-      <c r="I26"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="137"/>
-      <c r="B27" s="138"/>
-      <c r="C27" s="116"/>
-      <c r="D27" s="116"/>
-      <c r="E27" s="116"/>
-      <c r="F27" s="117"/>
-      <c r="I27"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="91"/>
-      <c r="B28" s="135"/>
-      <c r="C28" s="119"/>
-      <c r="D28" s="119"/>
-      <c r="E28" s="119"/>
-      <c r="F28" s="92"/>
       <c r="I28"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="136" t="s">
+      <c r="A29" s="137"/>
+      <c r="B29" s="138"/>
+      <c r="C29" s="118"/>
+      <c r="D29" s="116"/>
+      <c r="E29" s="116"/>
+      <c r="F29" s="117"/>
+      <c r="I29"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="91"/>
+      <c r="B30" s="135"/>
+      <c r="C30" s="119"/>
+      <c r="D30" s="119"/>
+      <c r="E30" s="119"/>
+      <c r="F30" s="92"/>
+      <c r="I30"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="136" t="s">
         <v>286</v>
       </c>
-      <c r="B29" s="126"/>
-      <c r="C29" s="133" t="s">
+      <c r="B31" s="126"/>
+      <c r="C31" s="133" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="133" t="s">
+      <c r="D31" s="133" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="133" t="s">
+      <c r="E31" s="133" t="s">
         <v>38</v>
       </c>
-      <c r="F29" s="134" t="s">
+      <c r="F31" s="134" t="s">
         <v>39</v>
-      </c>
-      <c r="I29"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="131"/>
-      <c r="B30" s="124" t="s">
-        <v>275</v>
-      </c>
-      <c r="C30" s="118"/>
-      <c r="D30" s="118"/>
-      <c r="E30" s="118"/>
-      <c r="F30" s="26"/>
-      <c r="I30"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="131"/>
-      <c r="B31" s="124" t="s">
-        <v>276</v>
-      </c>
-      <c r="C31" s="118" t="s">
-        <v>266</v>
-      </c>
-      <c r="D31" s="118" t="s">
-        <v>273</v>
-      </c>
-      <c r="E31" s="118" t="s">
-        <v>271</v>
-      </c>
-      <c r="F31" s="121" t="s">
-        <v>279</v>
       </c>
       <c r="I31"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="131"/>
       <c r="B32" s="124" t="s">
+        <v>275</v>
+      </c>
+      <c r="C32" s="118"/>
+      <c r="D32" s="118"/>
+      <c r="E32" s="118"/>
+      <c r="F32" s="26"/>
+      <c r="I32"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="131"/>
+      <c r="B33" s="124" t="s">
+        <v>276</v>
+      </c>
+      <c r="C33" s="118" t="s">
+        <v>266</v>
+      </c>
+      <c r="D33" s="187" t="s">
+        <v>350</v>
+      </c>
+      <c r="E33" s="118" t="s">
+        <v>271</v>
+      </c>
+      <c r="F33" s="121" t="s">
+        <v>279</v>
+      </c>
+      <c r="I33"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="131"/>
+      <c r="B34" s="124" t="s">
         <v>277</v>
       </c>
-      <c r="C32" s="118" t="s">
+      <c r="C34" s="118" t="s">
         <v>269</v>
       </c>
-      <c r="D32" s="118" t="s">
+      <c r="D34" s="118" t="s">
         <v>267</v>
       </c>
-      <c r="E32" s="118" t="s">
+      <c r="E34" s="118" t="s">
         <v>274</v>
       </c>
-      <c r="F32" s="121" t="s">
+      <c r="F34" s="121" t="s">
         <v>279</v>
       </c>
-      <c r="I32"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="132"/>
-      <c r="B33" s="127" t="s">
+      <c r="I34"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" s="132"/>
+      <c r="B35" s="127" t="s">
         <v>278</v>
       </c>
-      <c r="C33" s="119" t="s">
+      <c r="C35" s="119" t="s">
         <v>272</v>
       </c>
-      <c r="D33" s="119" t="s">
+      <c r="D35" s="119" t="s">
         <v>270</v>
       </c>
-      <c r="E33" s="119" t="s">
+      <c r="E35" s="119" t="s">
         <v>268</v>
       </c>
-      <c r="F33" s="122" t="s">
+      <c r="F35" s="122" t="s">
         <v>279</v>
       </c>
-      <c r="I33"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B34" s="11"/>
-      <c r="I34"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B35" s="11"/>
       <c r="I35"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>